<commit_message>
modified links on connection diagram
</commit_message>
<xml_diff>
--- a/Electrical/Arduino_ExternalConnections.xlsx
+++ b/Electrical/Arduino_ExternalConnections.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8777" yWindow="0" windowWidth="18523" windowHeight="10423" xr2:uid="{275B7CE7-B5D7-42A8-8D01-8AF01286FEB7}"/>
+    <workbookView xWindow="9874" yWindow="0" windowWidth="18523" windowHeight="10423" xr2:uid="{275B7CE7-B5D7-42A8-8D01-8AF01286FEB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Interface Type</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Serial (from the Pi)</t>
   </si>
   <si>
-    <t>pcie</t>
-  </si>
-  <si>
     <t>Motor &amp; Encoder</t>
   </si>
   <si>
@@ -180,6 +177,12 @@
   </si>
   <si>
     <t>6-pin screw terminal</t>
+  </si>
+  <si>
+    <t>Undecided.. PCIE?</t>
+  </si>
+  <si>
+    <t>see sparkfun arduino header kit</t>
   </si>
 </sst>
 </file>
@@ -273,7 +276,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -281,9 +284,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -295,7 +295,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -611,16 +611,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91353DA0-C921-4B81-83D7-9273390D1805}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="29.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.4609375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.69140625" customWidth="1"/>
     <col min="3" max="3" width="19.23046875" customWidth="1"/>
     <col min="4" max="4" width="10.921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="45" bestFit="1" customWidth="1"/>
@@ -647,37 +647,39 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
-      <c r="B3" s="10"/>
+      <c r="B3" s="9"/>
     </row>
     <row r="4" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>17</v>
+      <c r="B4" s="10" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
-      <c r="B5" s="11"/>
+      <c r="B5" s="10"/>
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>8</v>
@@ -700,94 +702,98 @@
     </row>
     <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3"/>
-      <c r="D9" s="12" t="s">
-        <v>22</v>
+      <c r="D9" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3"/>
-      <c r="D10" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>28</v>
+      <c r="D10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3"/>
-      <c r="D11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>29</v>
+      <c r="D11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3"/>
-      <c r="D12" s="12" t="s">
-        <v>24</v>
+      <c r="D12" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="5"/>
       <c r="D13" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3"/>
       <c r="D15" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>41</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3"/>
@@ -795,61 +801,98 @@
         <v>37</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3"/>
       <c r="D17" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="3"/>
       <c r="D18" s="4" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="5"/>
-      <c r="D19" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
+    <row r="19" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
+    </row>
+    <row r="20" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B26" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="7"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="E27" s="7"/>
+    </row>
+    <row r="26" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="3"/>
+      <c r="E26" s="10"/>
+    </row>
+    <row r="27" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="3"/>
+    </row>
+    <row r="34" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="3"/>
+    </row>
+    <row r="35" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="3"/>
+    </row>
+    <row r="36" spans="1:1" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="5"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D14" r:id="rId1" location="Supplier-Product-Code" xr:uid="{21440BA0-23A5-4604-A42D-7D1936A9B48B}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
organized and cleaned up connections document. just need 3 more connectors for the arduino shield
</commit_message>
<xml_diff>
--- a/Electrical/Arduino_ExternalConnections.xlsx
+++ b/Electrical/Arduino_ExternalConnections.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub_Local\2018\Electrical\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github_Local\2018\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9874" yWindow="0" windowWidth="18523" windowHeight="10423" xr2:uid="{275B7CE7-B5D7-42A8-8D01-8AF01286FEB7}"/>
+    <workbookView xWindow="10800" yWindow="0" windowWidth="18525" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
-  <si>
-    <t>Interface Type</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Signal Name</t>
   </si>
@@ -53,12 +50,6 @@
     <t>https://www.digikey.com/products/en?keywords=WM4824-ND</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/sullins-connector-solutions/PPTC202LFBN-RC/S6104-ND/807240</t>
-  </si>
-  <si>
-    <t>Sensor Link</t>
-  </si>
-  <si>
     <t>Arduino Shield Interface</t>
   </si>
   <si>
@@ -122,9 +113,6 @@
     <t>https://www.pololu.com/product/2824</t>
   </si>
   <si>
-    <t>Level Shifters (for encoder signals)</t>
-  </si>
-  <si>
     <t>https://www.sparkfun.com/products/12009</t>
   </si>
   <si>
@@ -176,20 +164,50 @@
     <t>Motor Controller Motor Power</t>
   </si>
   <si>
-    <t>6-pin screw terminal</t>
-  </si>
-  <si>
     <t>Undecided.. PCIE?</t>
   </si>
   <si>
     <t>see sparkfun arduino header kit</t>
+  </si>
+  <si>
+    <t>6-pin 0.2" spaced latched female header</t>
+  </si>
+  <si>
+    <t>Interface</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Level Shifters (for encoder A&amp;B)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">*note: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>use 18-gauge wire (10 A)</t>
+    </r>
+  </si>
+  <si>
+    <t>something that can handle 30A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,6 +223,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -214,7 +240,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -271,12 +297,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -287,7 +344,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -296,6 +352,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -610,289 +674,367 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91353DA0-C921-4B81-83D7-9273390D1805}">
-  <dimension ref="A1:F36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.69140625" customWidth="1"/>
-    <col min="3" max="3" width="19.23046875" customWidth="1"/>
-    <col min="4" max="4" width="10.921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.3046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="15"/>
+    </row>
+    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F7" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="7" t="s">
+    </row>
+    <row r="19" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="14"/>
+    </row>
+    <row r="20" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="13"/>
+    </row>
+    <row r="21" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="13"/>
+      <c r="D22" s="13"/>
+    </row>
+    <row r="23" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="13"/>
+      <c r="D23" s="13"/>
+    </row>
+    <row r="24" spans="1:6" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5"/>
+      <c r="B24" s="15"/>
+      <c r="D24" s="15"/>
+    </row>
+    <row r="25" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="5"/>
-      <c r="B3" s="9"/>
-    </row>
-    <row r="4" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="3"/>
-      <c r="B5" s="10"/>
-    </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="3"/>
-      <c r="D7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="3"/>
-      <c r="D9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="3"/>
-      <c r="D10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="3"/>
-      <c r="D11" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="3"/>
-      <c r="D12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="5"/>
-      <c r="D13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="6" t="s">
+      <c r="B25" s="16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="3"/>
-      <c r="D15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="12"/>
-    </row>
-    <row r="16" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="3"/>
-      <c r="D16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="3"/>
-      <c r="D17" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="4" t="s">
+      <c r="C25" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="3"/>
-      <c r="D18" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="5"/>
-    </row>
-    <row r="25" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="D25" s="14"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
-      <c r="E26" s="10"/>
-    </row>
-    <row r="27" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
-    </row>
-    <row r="28" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="13"/>
+      <c r="D27" s="13"/>
+    </row>
+    <row r="28" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="13"/>
+      <c r="D28" s="13"/>
+    </row>
+    <row r="29" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
-    </row>
-    <row r="30" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B29" s="13"/>
+      <c r="D29" s="13"/>
+    </row>
+    <row r="30" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
-    </row>
-    <row r="31" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="13"/>
+      <c r="D30" s="13"/>
+    </row>
+    <row r="31" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
-    </row>
-    <row r="32" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="13"/>
+      <c r="D31" s="13"/>
+    </row>
+    <row r="32" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
-    </row>
-    <row r="33" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="13"/>
+      <c r="D32" s="13"/>
+    </row>
+    <row r="33" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
-    </row>
-    <row r="34" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="13"/>
+      <c r="D33" s="13"/>
+    </row>
+    <row r="34" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
-    </row>
-    <row r="35" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B34" s="13"/>
+      <c r="D34" s="13"/>
+    </row>
+    <row r="35" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
-    </row>
-    <row r="36" spans="1:1" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B35" s="13"/>
+      <c r="D35" s="13"/>
+    </row>
+    <row r="36" spans="1:4" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
+      <c r="B36" s="15"/>
+      <c r="D36" s="15"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1"/>
+    <hyperlink ref="D8" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished all connectors. now to do schematic and footprint association
</commit_message>
<xml_diff>
--- a/Electrical/Arduino_ExternalConnections.xlsx
+++ b/Electrical/Arduino_ExternalConnections.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13590" yWindow="0" windowWidth="18525" windowHeight="10425"/>
+    <workbookView xWindow="14520" yWindow="0" windowWidth="18525" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="98">
   <si>
     <t>Signal Name</t>
   </si>
@@ -323,13 +323,7 @@
     <t>"</t>
   </si>
   <si>
-    <t>undecided</t>
-  </si>
-  <si>
     <t>3x 2-pin 0.2" spaced female header</t>
-  </si>
-  <si>
-    <t>Undecided.. PCIE? (20A)</t>
   </si>
   <si>
     <r>
@@ -343,15 +337,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>use 18-gauge wire (20 A)</t>
+      <t>use 16-gauge wire(18 A)</t>
     </r>
+  </si>
+  <si>
+    <t>2-pin blade connector (rated to 18A)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,25 +379,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="15">
@@ -554,10 +539,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -661,9 +645,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -694,9 +675,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1027,7 +1008,7 @@
     <col min="4" max="4" width="7.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" style="42" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.28515625" style="31" bestFit="1" customWidth="1"/>
   </cols>
@@ -1071,7 +1052,7 @@
       <c r="C2" s="19">
         <v>1</v>
       </c>
-      <c r="D2" s="50"/>
+      <c r="D2" s="49"/>
       <c r="G2" s="37" t="s">
         <v>88</v>
       </c>
@@ -1088,7 +1069,7 @@
         <v>90</v>
       </c>
       <c r="C3" s="21"/>
-      <c r="D3" s="54"/>
+      <c r="D3" s="53"/>
       <c r="G3" s="38" t="s">
         <v>89</v>
       </c>
@@ -1103,7 +1084,7 @@
       <c r="A4" s="3"/>
       <c r="B4" s="9"/>
       <c r="C4" s="21"/>
-      <c r="D4" s="54"/>
+      <c r="D4" s="53"/>
       <c r="G4" s="3" t="s">
         <v>91</v>
       </c>
@@ -1117,7 +1098,7 @@
     <row r="5" spans="1:9" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="C5" s="20"/>
-      <c r="D5" s="51"/>
+      <c r="D5" s="50"/>
       <c r="G5" s="5" t="s">
         <v>92</v>
       </c>
@@ -1138,7 +1119,7 @@
       <c r="C6" s="21">
         <v>1</v>
       </c>
-      <c r="D6" s="52"/>
+      <c r="D6" s="51"/>
       <c r="E6" s="4" t="s">
         <v>74</v>
       </c>
@@ -1148,15 +1129,15 @@
       <c r="G6" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="H6" s="49" t="s">
-        <v>95</v>
+      <c r="H6" s="59" t="s">
+        <v>72</v>
       </c>
       <c r="I6" s="31"/>
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="C7" s="21"/>
-      <c r="D7" s="53"/>
+      <c r="D7" s="52"/>
       <c r="E7" s="4" t="s">
         <v>75</v>
       </c>
@@ -1164,7 +1145,7 @@
         <v>46</v>
       </c>
       <c r="G7" s="39" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H7" s="42"/>
       <c r="I7" s="31"/>
@@ -1179,7 +1160,7 @@
       <c r="C8" s="19">
         <v>1</v>
       </c>
-      <c r="D8" s="50"/>
+      <c r="D8" s="49"/>
       <c r="E8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1197,7 +1178,7 @@
     <row r="9" spans="1:9" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="C9" s="21"/>
-      <c r="D9" s="51"/>
+      <c r="D9" s="50"/>
       <c r="E9" s="4" t="s">
         <v>1</v>
       </c>
@@ -1218,7 +1199,7 @@
       <c r="C10" s="19">
         <v>6</v>
       </c>
-      <c r="D10" s="50"/>
+      <c r="D10" s="49"/>
       <c r="E10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1236,7 +1217,7 @@
     <row r="11" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="C11" s="21"/>
-      <c r="D11" s="54"/>
+      <c r="D11" s="53"/>
       <c r="E11" s="8" t="s">
         <v>13</v>
       </c>
@@ -1250,7 +1231,7 @@
     <row r="12" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="C12" s="21"/>
-      <c r="D12" s="54"/>
+      <c r="D12" s="53"/>
       <c r="E12" s="8" t="s">
         <v>11</v>
       </c>
@@ -1264,7 +1245,7 @@
     <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="C13" s="21"/>
-      <c r="D13" s="54"/>
+      <c r="D13" s="53"/>
       <c r="E13" s="8" t="s">
         <v>14</v>
       </c>
@@ -1278,7 +1259,7 @@
     <row r="14" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="C14" s="21"/>
-      <c r="D14" s="54"/>
+      <c r="D14" s="53"/>
       <c r="E14" s="8" t="s">
         <v>15</v>
       </c>
@@ -1292,7 +1273,7 @@
     <row r="15" spans="1:9" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="C15" s="20"/>
-      <c r="D15" s="51"/>
+      <c r="D15" s="50"/>
       <c r="E15" s="6" t="s">
         <v>16</v>
       </c>
@@ -1313,7 +1294,7 @@
       <c r="C16" s="32">
         <v>3</v>
       </c>
-      <c r="D16" s="59" t="s">
+      <c r="D16" s="58" t="s">
         <v>86</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -1333,7 +1314,7 @@
     <row r="17" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="C17" s="21"/>
-      <c r="D17" s="56"/>
+      <c r="D17" s="55"/>
       <c r="E17" s="4" t="s">
         <v>22</v>
       </c>
@@ -1347,7 +1328,7 @@
     <row r="18" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="C18" s="21"/>
-      <c r="D18" s="56"/>
+      <c r="D18" s="55"/>
       <c r="E18" s="4" t="s">
         <v>23</v>
       </c>
@@ -1361,7 +1342,7 @@
     <row r="19" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="C19" s="21"/>
-      <c r="D19" s="56"/>
+      <c r="D19" s="55"/>
       <c r="E19" s="4" t="s">
         <v>24</v>
       </c>
@@ -1376,7 +1357,7 @@
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="21"/>
-      <c r="D20" s="57"/>
+      <c r="D20" s="56"/>
       <c r="E20" s="15" t="s">
         <v>3</v>
       </c>
@@ -1391,7 +1372,7 @@
       <c r="A21" s="3"/>
       <c r="B21" s="25"/>
       <c r="C21" s="40"/>
-      <c r="D21" s="55" t="s">
+      <c r="D21" s="54" t="s">
         <v>85</v>
       </c>
       <c r="E21" s="12" t="s">
@@ -1401,7 +1382,7 @@
         <v>44</v>
       </c>
       <c r="G21" s="36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>72</v>
@@ -1411,7 +1392,7 @@
     <row r="22" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="C22" s="21"/>
-      <c r="D22" s="56"/>
+      <c r="D22" s="55"/>
       <c r="E22" s="8" t="s">
         <v>37</v>
       </c>
@@ -1427,7 +1408,7 @@
     <row r="23" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="C23" s="21"/>
-      <c r="D23" s="56"/>
+      <c r="D23" s="55"/>
       <c r="E23" s="8" t="s">
         <v>38</v>
       </c>
@@ -1435,7 +1416,7 @@
         <v>78</v>
       </c>
       <c r="G23" s="36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H23" s="45" t="s">
         <v>94</v>
@@ -1445,7 +1426,7 @@
     <row r="24" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="C24" s="21"/>
-      <c r="D24" s="56"/>
+      <c r="D24" s="55"/>
       <c r="E24" s="8" t="s">
         <v>39</v>
       </c>
@@ -1459,7 +1440,7 @@
     <row r="25" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="C25" s="21"/>
-      <c r="D25" s="56"/>
+      <c r="D25" s="55"/>
       <c r="E25" s="8" t="s">
         <v>40</v>
       </c>
@@ -1467,7 +1448,7 @@
         <v>45</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H25" s="42" t="s">
         <v>94</v>
@@ -1477,7 +1458,7 @@
     <row r="26" spans="1:9" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="C26" s="20"/>
-      <c r="D26" s="58"/>
+      <c r="D26" s="57"/>
       <c r="E26" s="6" t="s">
         <v>41</v>
       </c>
@@ -1498,7 +1479,7 @@
       <c r="C27" s="32">
         <v>3</v>
       </c>
-      <c r="D27" s="55" t="s">
+      <c r="D27" s="54" t="s">
         <v>68</v>
       </c>
       <c r="E27" s="13" t="s">
@@ -1518,7 +1499,7 @@
     <row r="28" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="C28" s="33"/>
-      <c r="D28" s="56"/>
+      <c r="D28" s="55"/>
       <c r="E28" s="8" t="s">
         <v>49</v>
       </c>
@@ -1532,7 +1513,7 @@
     <row r="29" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="C29" s="21"/>
-      <c r="D29" s="56"/>
+      <c r="D29" s="55"/>
       <c r="E29" s="8" t="s">
         <v>50</v>
       </c>
@@ -1546,7 +1527,7 @@
     <row r="30" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="C30" s="21"/>
-      <c r="D30" s="56"/>
+      <c r="D30" s="55"/>
       <c r="E30" s="8" t="s">
         <v>3</v>
       </c>
@@ -1560,7 +1541,7 @@
     <row r="31" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="C31" s="21"/>
-      <c r="D31" s="56"/>
+      <c r="D31" s="55"/>
       <c r="E31" s="8" t="s">
         <v>51</v>
       </c>
@@ -1575,7 +1556,7 @@
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="21"/>
-      <c r="D32" s="57"/>
+      <c r="D32" s="56"/>
       <c r="E32" s="16" t="s">
         <v>52</v>
       </c>
@@ -1589,7 +1570,7 @@
     <row r="33" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="C33" s="21"/>
-      <c r="D33" s="55" t="s">
+      <c r="D33" s="54" t="s">
         <v>69</v>
       </c>
       <c r="E33" s="8" t="s">
@@ -1609,7 +1590,7 @@
     <row r="34" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="C34" s="21"/>
-      <c r="D34" s="56"/>
+      <c r="D34" s="55"/>
       <c r="E34" s="8" t="s">
         <v>57</v>
       </c>
@@ -1623,7 +1604,7 @@
     <row r="35" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="C35" s="21"/>
-      <c r="D35" s="56"/>
+      <c r="D35" s="55"/>
       <c r="E35" s="8" t="s">
         <v>58</v>
       </c>
@@ -1637,7 +1618,7 @@
     <row r="36" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="C36" s="21"/>
-      <c r="D36" s="56"/>
+      <c r="D36" s="55"/>
       <c r="E36" s="8" t="s">
         <v>3</v>
       </c>
@@ -1651,7 +1632,7 @@
     <row r="37" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="C37" s="21"/>
-      <c r="D37" s="56"/>
+      <c r="D37" s="55"/>
       <c r="E37" s="8" t="s">
         <v>59</v>
       </c>
@@ -1665,7 +1646,7 @@
     <row r="38" spans="1:9" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="C38" s="20"/>
-      <c r="D38" s="58"/>
+      <c r="D38" s="57"/>
       <c r="E38" s="6" t="s">
         <v>60</v>
       </c>
@@ -1701,8 +1682,9 @@
     <hyperlink ref="H4" r:id="rId11"/>
     <hyperlink ref="H5" r:id="rId12"/>
     <hyperlink ref="H21" r:id="rId13"/>
+    <hyperlink ref="H6" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
starting pi cape schematic
</commit_message>
<xml_diff>
--- a/Electrical/Arduino_ExternalConnections.xlsx
+++ b/Electrical/Arduino_ExternalConnections.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="0" windowWidth="18525" windowHeight="10425"/>
+    <workbookView xWindow="16380" yWindow="0" windowWidth="18525" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -341,7 +341,7 @@
     </r>
   </si>
   <si>
-    <t>2-pin blade connector (rated to 18A)</t>
+    <t>2-pin 0.295" blade connector (rated to 18A)</t>
   </si>
 </sst>
 </file>
@@ -543,7 +543,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -645,6 +645,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -675,7 +677,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -997,7 +998,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,7 +1009,7 @@
     <col min="4" max="4" width="7.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" style="42" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.28515625" style="31" bestFit="1" customWidth="1"/>
   </cols>
@@ -1052,7 +1053,7 @@
       <c r="C2" s="19">
         <v>1</v>
       </c>
-      <c r="D2" s="49"/>
+      <c r="D2" s="51"/>
       <c r="G2" s="37" t="s">
         <v>88</v>
       </c>
@@ -1069,7 +1070,7 @@
         <v>90</v>
       </c>
       <c r="C3" s="21"/>
-      <c r="D3" s="53"/>
+      <c r="D3" s="55"/>
       <c r="G3" s="38" t="s">
         <v>89</v>
       </c>
@@ -1084,7 +1085,7 @@
       <c r="A4" s="3"/>
       <c r="B4" s="9"/>
       <c r="C4" s="21"/>
-      <c r="D4" s="53"/>
+      <c r="D4" s="55"/>
       <c r="G4" s="3" t="s">
         <v>91</v>
       </c>
@@ -1098,7 +1099,7 @@
     <row r="5" spans="1:9" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="C5" s="20"/>
-      <c r="D5" s="50"/>
+      <c r="D5" s="52"/>
       <c r="G5" s="5" t="s">
         <v>92</v>
       </c>
@@ -1119,17 +1120,17 @@
       <c r="C6" s="21">
         <v>1</v>
       </c>
-      <c r="D6" s="51"/>
+      <c r="D6" s="53"/>
       <c r="E6" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="H6" s="59" t="s">
+      <c r="H6" s="49" t="s">
         <v>72</v>
       </c>
       <c r="I6" s="31"/>
@@ -1137,7 +1138,7 @@
     <row r="7" spans="1:9" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="C7" s="21"/>
-      <c r="D7" s="52"/>
+      <c r="D7" s="54"/>
       <c r="E7" s="4" t="s">
         <v>75</v>
       </c>
@@ -1160,7 +1161,7 @@
       <c r="C8" s="19">
         <v>1</v>
       </c>
-      <c r="D8" s="49"/>
+      <c r="D8" s="51"/>
       <c r="E8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1178,7 +1179,7 @@
     <row r="9" spans="1:9" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="C9" s="21"/>
-      <c r="D9" s="50"/>
+      <c r="D9" s="52"/>
       <c r="E9" s="4" t="s">
         <v>1</v>
       </c>
@@ -1199,7 +1200,7 @@
       <c r="C10" s="19">
         <v>6</v>
       </c>
-      <c r="D10" s="49"/>
+      <c r="D10" s="51"/>
       <c r="E10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1217,7 +1218,7 @@
     <row r="11" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="C11" s="21"/>
-      <c r="D11" s="53"/>
+      <c r="D11" s="55"/>
       <c r="E11" s="8" t="s">
         <v>13</v>
       </c>
@@ -1231,7 +1232,7 @@
     <row r="12" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="C12" s="21"/>
-      <c r="D12" s="53"/>
+      <c r="D12" s="55"/>
       <c r="E12" s="8" t="s">
         <v>11</v>
       </c>
@@ -1245,7 +1246,7 @@
     <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="C13" s="21"/>
-      <c r="D13" s="53"/>
+      <c r="D13" s="55"/>
       <c r="E13" s="8" t="s">
         <v>14</v>
       </c>
@@ -1259,7 +1260,7 @@
     <row r="14" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="C14" s="21"/>
-      <c r="D14" s="53"/>
+      <c r="D14" s="55"/>
       <c r="E14" s="8" t="s">
         <v>15</v>
       </c>
@@ -1273,7 +1274,7 @@
     <row r="15" spans="1:9" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="C15" s="20"/>
-      <c r="D15" s="50"/>
+      <c r="D15" s="52"/>
       <c r="E15" s="6" t="s">
         <v>16</v>
       </c>
@@ -1294,7 +1295,7 @@
       <c r="C16" s="32">
         <v>3</v>
       </c>
-      <c r="D16" s="58" t="s">
+      <c r="D16" s="60" t="s">
         <v>86</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -1314,7 +1315,7 @@
     <row r="17" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="C17" s="21"/>
-      <c r="D17" s="55"/>
+      <c r="D17" s="57"/>
       <c r="E17" s="4" t="s">
         <v>22</v>
       </c>
@@ -1328,7 +1329,7 @@
     <row r="18" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="C18" s="21"/>
-      <c r="D18" s="55"/>
+      <c r="D18" s="57"/>
       <c r="E18" s="4" t="s">
         <v>23</v>
       </c>
@@ -1342,7 +1343,7 @@
     <row r="19" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="C19" s="21"/>
-      <c r="D19" s="55"/>
+      <c r="D19" s="57"/>
       <c r="E19" s="4" t="s">
         <v>24</v>
       </c>
@@ -1357,7 +1358,7 @@
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="21"/>
-      <c r="D20" s="56"/>
+      <c r="D20" s="58"/>
       <c r="E20" s="15" t="s">
         <v>3</v>
       </c>
@@ -1372,7 +1373,7 @@
       <c r="A21" s="3"/>
       <c r="B21" s="25"/>
       <c r="C21" s="40"/>
-      <c r="D21" s="54" t="s">
+      <c r="D21" s="56" t="s">
         <v>85</v>
       </c>
       <c r="E21" s="12" t="s">
@@ -1392,7 +1393,7 @@
     <row r="22" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="C22" s="21"/>
-      <c r="D22" s="55"/>
+      <c r="D22" s="57"/>
       <c r="E22" s="8" t="s">
         <v>37</v>
       </c>
@@ -1408,7 +1409,7 @@
     <row r="23" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="C23" s="21"/>
-      <c r="D23" s="55"/>
+      <c r="D23" s="57"/>
       <c r="E23" s="8" t="s">
         <v>38</v>
       </c>
@@ -1426,7 +1427,7 @@
     <row r="24" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="C24" s="21"/>
-      <c r="D24" s="55"/>
+      <c r="D24" s="57"/>
       <c r="E24" s="8" t="s">
         <v>39</v>
       </c>
@@ -1440,7 +1441,7 @@
     <row r="25" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="C25" s="21"/>
-      <c r="D25" s="55"/>
+      <c r="D25" s="57"/>
       <c r="E25" s="8" t="s">
         <v>40</v>
       </c>
@@ -1458,7 +1459,7 @@
     <row r="26" spans="1:9" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="C26" s="20"/>
-      <c r="D26" s="57"/>
+      <c r="D26" s="59"/>
       <c r="E26" s="6" t="s">
         <v>41</v>
       </c>
@@ -1479,7 +1480,7 @@
       <c r="C27" s="32">
         <v>3</v>
       </c>
-      <c r="D27" s="54" t="s">
+      <c r="D27" s="56" t="s">
         <v>68</v>
       </c>
       <c r="E27" s="13" t="s">
@@ -1499,7 +1500,7 @@
     <row r="28" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="C28" s="33"/>
-      <c r="D28" s="55"/>
+      <c r="D28" s="57"/>
       <c r="E28" s="8" t="s">
         <v>49</v>
       </c>
@@ -1513,7 +1514,7 @@
     <row r="29" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="C29" s="21"/>
-      <c r="D29" s="55"/>
+      <c r="D29" s="57"/>
       <c r="E29" s="8" t="s">
         <v>50</v>
       </c>
@@ -1527,7 +1528,7 @@
     <row r="30" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="C30" s="21"/>
-      <c r="D30" s="55"/>
+      <c r="D30" s="57"/>
       <c r="E30" s="8" t="s">
         <v>3</v>
       </c>
@@ -1541,7 +1542,7 @@
     <row r="31" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="C31" s="21"/>
-      <c r="D31" s="55"/>
+      <c r="D31" s="57"/>
       <c r="E31" s="8" t="s">
         <v>51</v>
       </c>
@@ -1556,7 +1557,7 @@
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="21"/>
-      <c r="D32" s="56"/>
+      <c r="D32" s="58"/>
       <c r="E32" s="16" t="s">
         <v>52</v>
       </c>
@@ -1570,7 +1571,7 @@
     <row r="33" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="C33" s="21"/>
-      <c r="D33" s="54" t="s">
+      <c r="D33" s="56" t="s">
         <v>69</v>
       </c>
       <c r="E33" s="8" t="s">
@@ -1590,7 +1591,7 @@
     <row r="34" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="C34" s="21"/>
-      <c r="D34" s="55"/>
+      <c r="D34" s="57"/>
       <c r="E34" s="8" t="s">
         <v>57</v>
       </c>
@@ -1604,7 +1605,7 @@
     <row r="35" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="C35" s="21"/>
-      <c r="D35" s="55"/>
+      <c r="D35" s="57"/>
       <c r="E35" s="8" t="s">
         <v>58</v>
       </c>
@@ -1618,7 +1619,7 @@
     <row r="36" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="C36" s="21"/>
-      <c r="D36" s="55"/>
+      <c r="D36" s="57"/>
       <c r="E36" s="8" t="s">
         <v>3</v>
       </c>
@@ -1632,7 +1633,7 @@
     <row r="37" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="C37" s="21"/>
-      <c r="D37" s="55"/>
+      <c r="D37" s="57"/>
       <c r="E37" s="8" t="s">
         <v>59</v>
       </c>
@@ -1646,7 +1647,7 @@
     <row r="38" spans="1:9" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="C38" s="20"/>
-      <c r="D38" s="57"/>
+      <c r="D38" s="59"/>
       <c r="E38" s="6" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
updated Pi and Arduino external connection. Finished base Pi schematic
</commit_message>
<xml_diff>
--- a/Electrical/Arduino_ExternalConnections.xlsx
+++ b/Electrical/Arduino_ExternalConnections.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github_Local\2018\Electrical\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub_Local\2018\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16380" yWindow="0" windowWidth="18525" windowHeight="10425"/>
+    <workbookView xWindow="17477" yWindow="0" windowWidth="18523" windowHeight="10423" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="101">
   <si>
     <t>Signal Name</t>
   </si>
@@ -47,15 +47,6 @@
     <t>Connector</t>
   </si>
   <si>
-    <t>Receive</t>
-  </si>
-  <si>
-    <t>Transmit</t>
-  </si>
-  <si>
-    <t>Serial (from the Pi)</t>
-  </si>
-  <si>
     <t>Motor &amp; Encoder</t>
   </si>
   <si>
@@ -114,9 +105,6 @@
   </si>
   <si>
     <t>motor 2 speed</t>
-  </si>
-  <si>
-    <t>2-pin female latched header</t>
   </si>
   <si>
     <t>6-pin female latched header</t>
@@ -281,9 +269,6 @@
     <t>Motor Ground (from motor controller)</t>
   </si>
   <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>due</t>
   </si>
   <si>
@@ -343,11 +328,35 @@
   <si>
     <t>2-pin 0.295" blade connector (rated to 18A)</t>
   </si>
+  <si>
+    <t>Pi Interface</t>
+  </si>
+  <si>
+    <t>serial</t>
+  </si>
+  <si>
+    <t>PWR_5V</t>
+  </si>
+  <si>
+    <t>4-pin female latched 0.1" header</t>
+  </si>
+  <si>
+    <t>5V to power the Pi (pin 2)</t>
+  </si>
+  <si>
+    <t>Ground for Pi (pin 6)</t>
+  </si>
+  <si>
+    <t>Arduino's Receive (connect to Pi's Tx)</t>
+  </si>
+  <si>
+    <t>Arduino's Transmit (connect to Pi's Rx)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -543,7 +552,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -656,9 +665,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -677,6 +683,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -991,41 +1007,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="27.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.15234375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.15234375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.3046875" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.53515625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="42" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.3828125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.69140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.53515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.3046875" style="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="22" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="22" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="26" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E1" s="22" t="s">
         <v>0</v>
@@ -1037,653 +1053,680 @@
         <v>6</v>
       </c>
       <c r="H1" s="27" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="I1" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>82</v>
       </c>
       <c r="C2" s="19">
         <v>1</v>
       </c>
       <c r="D2" s="51"/>
       <c r="G2" s="37" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I2" s="29">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="47"/>
       <c r="B3" s="9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C3" s="21"/>
-      <c r="D3" s="55"/>
+      <c r="D3" s="54"/>
       <c r="G3" s="38" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I3" s="31">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3"/>
       <c r="B4" s="9"/>
       <c r="C4" s="21"/>
-      <c r="D4" s="55"/>
+      <c r="D4" s="54"/>
       <c r="G4" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I4" s="31">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
       <c r="C5" s="20"/>
       <c r="D5" s="52"/>
       <c r="G5" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H5" s="48" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I5" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C6" s="21">
         <v>1</v>
       </c>
       <c r="D6" s="53"/>
       <c r="E6" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="G6" s="50" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="H6" s="49" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I6" s="31"/>
     </row>
-    <row r="7" spans="1:9" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="3"/>
       <c r="C7" s="21"/>
-      <c r="D7" s="54"/>
+      <c r="D7" s="60"/>
       <c r="E7" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G7" s="39" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H7" s="42"/>
       <c r="I7" s="31"/>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="C8" s="19">
         <v>1</v>
       </c>
-      <c r="D8" s="51"/>
+      <c r="D8" s="59" t="s">
+        <v>80</v>
+      </c>
       <c r="E8" s="2" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>30</v>
+        <v>97</v>
+      </c>
+      <c r="G8" s="63" t="s">
+        <v>96</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I8" s="29"/>
     </row>
-    <row r="9" spans="1:9" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3"/>
       <c r="C9" s="21"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="3"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="39"/>
       <c r="H9" s="42"/>
       <c r="I9" s="31"/>
     </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="19">
+    <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="3"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="31"/>
+    </row>
+    <row r="11" spans="1:9" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="5"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="30"/>
+    </row>
+    <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="19">
         <v>6</v>
       </c>
-      <c r="D10" s="51"/>
-      <c r="E10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G10" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="I10" s="29"/>
-    </row>
-    <row r="11" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="31"/>
-    </row>
-    <row r="12" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="31"/>
-    </row>
-    <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="51"/>
+      <c r="E12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="I12" s="29"/>
+    </row>
+    <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3"/>
       <c r="C13" s="21"/>
-      <c r="D13" s="55"/>
+      <c r="D13" s="54"/>
       <c r="E13" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="42"/>
       <c r="I13" s="31"/>
     </row>
-    <row r="14" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3"/>
       <c r="C14" s="21"/>
-      <c r="D14" s="55"/>
+      <c r="D14" s="54"/>
       <c r="E14" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>20</v>
+        <v>8</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="42"/>
       <c r="I14" s="31"/>
     </row>
-    <row r="15" spans="1:9" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="6" t="s">
+    <row r="15" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="3"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="31"/>
+    </row>
+    <row r="16" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="3"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="31"/>
+    </row>
+    <row r="17" spans="1:9" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="5"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="30"/>
-    </row>
-    <row r="16" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="32">
+      <c r="G17" s="5"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="30"/>
+    </row>
+    <row r="18" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="32">
         <v>3</v>
       </c>
-      <c r="D16" s="60" t="s">
-        <v>86</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H16" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="I16" s="29"/>
-    </row>
-    <row r="17" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="4" t="s">
+      <c r="D18" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="31"/>
-    </row>
-    <row r="18" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="31"/>
-    </row>
-    <row r="19" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" s="29"/>
+    </row>
+    <row r="19" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A19" s="3"/>
       <c r="C19" s="21"/>
-      <c r="D19" s="57"/>
+      <c r="D19" s="56"/>
       <c r="E19" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="42"/>
       <c r="I19" s="31"/>
     </row>
-    <row r="20" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
       <c r="C20" s="21"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="G20" s="34"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="35"/>
-    </row>
-    <row r="21" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="56"/>
+      <c r="E20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="31"/>
+    </row>
+    <row r="21" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G21" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="I21" s="46"/>
-    </row>
-    <row r="22" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="21"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="31"/>
+    </row>
+    <row r="22" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3"/>
+      <c r="B22" s="4"/>
       <c r="C22" s="21"/>
       <c r="D22" s="57"/>
-      <c r="E22" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G22" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22" s="42"/>
-      <c r="I22" s="31"/>
-    </row>
-    <row r="23" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E22" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="34"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="35"/>
+    </row>
+    <row r="23" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>78</v>
+      <c r="B23" s="25"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>40</v>
       </c>
       <c r="G23" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="H23" s="45" t="s">
-        <v>94</v>
+        <v>90</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="I23" s="46"/>
     </row>
-    <row r="24" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3"/>
       <c r="C24" s="21"/>
-      <c r="D24" s="57"/>
+      <c r="D24" s="56"/>
       <c r="E24" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="G24" s="34"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="35"/>
-    </row>
-    <row r="25" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G24" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24" s="42"/>
+      <c r="I24" s="31"/>
+    </row>
+    <row r="25" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3"/>
       <c r="C25" s="21"/>
-      <c r="D25" s="57"/>
+      <c r="D25" s="56"/>
       <c r="E25" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F25" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G25" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="H25" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="I25" s="46"/>
+    </row>
+    <row r="26" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="3"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="34"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="35"/>
+    </row>
+    <row r="27" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="3"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H27" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="I27" s="31"/>
+    </row>
+    <row r="28" spans="1:9" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="5"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G28" s="5"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="30"/>
+    </row>
+    <row r="29" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="32">
+        <v>3</v>
+      </c>
+      <c r="D29" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="I29" s="46"/>
+    </row>
+    <row r="30" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="3"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="H25" s="42" t="s">
-        <v>94</v>
-      </c>
-      <c r="I25" s="31"/>
-    </row>
-    <row r="26" spans="1:9" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="59"/>
-      <c r="E26" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G26" s="5"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="30"/>
-    </row>
-    <row r="27" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B27" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" s="32">
-        <v>3</v>
-      </c>
-      <c r="D27" s="56" t="s">
-        <v>68</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H27" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="I27" s="46"/>
-    </row>
-    <row r="28" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G28" s="3"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="31"/>
-    </row>
-    <row r="29" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="8" t="s">
+      <c r="F30" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="G29" s="3"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="31"/>
-    </row>
-    <row r="30" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>5</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="42"/>
       <c r="I30" s="31"/>
     </row>
-    <row r="31" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="3"/>
       <c r="C31" s="21"/>
-      <c r="D31" s="57"/>
+      <c r="D31" s="56"/>
       <c r="E31" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>55</v>
+        <v>46</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="42"/>
       <c r="I31" s="31"/>
     </row>
-    <row r="32" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A32" s="3"/>
-      <c r="B32" s="4"/>
       <c r="C32" s="21"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F32" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="G32" s="34"/>
-      <c r="H32" s="44"/>
-      <c r="I32" s="35"/>
-    </row>
-    <row r="33" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="56"/>
+      <c r="E32" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="3"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="31"/>
+    </row>
+    <row r="33" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A33" s="3"/>
       <c r="C33" s="21"/>
-      <c r="D33" s="56" t="s">
-        <v>69</v>
-      </c>
+      <c r="D33" s="56"/>
       <c r="E33" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G33" s="36" t="s">
-        <v>93</v>
-      </c>
-      <c r="H33" s="45" t="s">
-        <v>94</v>
-      </c>
-      <c r="I33" s="46"/>
-    </row>
-    <row r="34" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G33" s="3"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="31"/>
+    </row>
+    <row r="34" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A34" s="3"/>
+      <c r="B34" s="4"/>
       <c r="C34" s="21"/>
       <c r="D34" s="57"/>
-      <c r="E34" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G34" s="3"/>
-      <c r="H34" s="42"/>
-      <c r="I34" s="31"/>
-    </row>
-    <row r="35" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E34" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="G34" s="34"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="35"/>
+    </row>
+    <row r="35" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A35" s="3"/>
       <c r="C35" s="21"/>
-      <c r="D35" s="57"/>
+      <c r="D35" s="55" t="s">
+        <v>65</v>
+      </c>
       <c r="E35" s="8" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="G35" s="3"/>
-      <c r="H35" s="42"/>
-      <c r="I35" s="31"/>
-    </row>
-    <row r="36" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="G35" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="H35" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="I35" s="46"/>
+    </row>
+    <row r="36" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="3"/>
       <c r="C36" s="21"/>
-      <c r="D36" s="57"/>
+      <c r="D36" s="56"/>
       <c r="E36" s="8" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="42"/>
       <c r="I36" s="31"/>
     </row>
-    <row r="37" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A37" s="3"/>
       <c r="C37" s="21"/>
-      <c r="D37" s="57"/>
+      <c r="D37" s="56"/>
       <c r="E37" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="42"/>
       <c r="I37" s="31"/>
     </row>
-    <row r="38" spans="1:9" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="5"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="59"/>
-      <c r="E38" s="6" t="s">
+    <row r="38" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="3"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" s="3"/>
+      <c r="H38" s="42"/>
+      <c r="I38" s="31"/>
+    </row>
+    <row r="39" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="3"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G39" s="3"/>
+      <c r="H39" s="42"/>
+      <c r="I39" s="31"/>
+    </row>
+    <row r="40" spans="1:9" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="5"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="58"/>
+      <c r="E40" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F40" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F38" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G38" s="5"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="30"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="41"/>
+      <c r="I40" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="D8:D9"/>
+  <mergeCells count="9">
+    <mergeCell ref="D10:D11"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D2:D5"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="D33:D38"/>
-    <mergeCell ref="D16:D20"/>
-    <mergeCell ref="D21:D26"/>
-    <mergeCell ref="D10:D15"/>
+    <mergeCell ref="D29:D34"/>
+    <mergeCell ref="D35:D40"/>
+    <mergeCell ref="D18:D22"/>
+    <mergeCell ref="D23:D28"/>
+    <mergeCell ref="D12:D17"/>
+    <mergeCell ref="D8:D9"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H8" r:id="rId1"/>
-    <hyperlink ref="H10" r:id="rId2"/>
-    <hyperlink ref="B10" r:id="rId3" display="pPololu"/>
-    <hyperlink ref="B16" r:id="rId4" location="Supplier-Product-Code" display="Robotshop"/>
-    <hyperlink ref="B27" r:id="rId5" display="Sparkfun"/>
-    <hyperlink ref="B2" r:id="rId6"/>
-    <hyperlink ref="H27" r:id="rId7"/>
-    <hyperlink ref="H2" r:id="rId8"/>
-    <hyperlink ref="H3" r:id="rId9"/>
-    <hyperlink ref="B3" r:id="rId10"/>
-    <hyperlink ref="H4" r:id="rId11"/>
-    <hyperlink ref="H5" r:id="rId12"/>
-    <hyperlink ref="H21" r:id="rId13"/>
-    <hyperlink ref="H6" r:id="rId14"/>
+    <hyperlink ref="H12" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B12" r:id="rId2" display="pPololu" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B18" r:id="rId3" location="Supplier-Product-Code" display="Robotshop" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B29" r:id="rId4" display="Sparkfun" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H29" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H2" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H3" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B3" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="H4" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="H5" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="H23" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="H6" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="H8" r:id="rId14" xr:uid="{0E01A5F4-00F9-40BD-990F-C3B6F2273C64}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId15"/>

</xml_diff>

<commit_message>
moved imu from pi to arduino on excel sheets
</commit_message>
<xml_diff>
--- a/Electrical/Arduino_ExternalConnections.xlsx
+++ b/Electrical/Arduino_ExternalConnections.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub_Local\2018\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC542083-4E6B-4F13-8530-56EB9B000040}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17477" yWindow="0" windowWidth="18523" windowHeight="10423" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18574" yWindow="0" windowWidth="18523" windowHeight="10423" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="130">
   <si>
     <t>Signal Name</t>
   </si>
@@ -351,6 +352,95 @@
   </si>
   <si>
     <t>Arduino's Transmit (connect to Pi's Rx)</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>VDD/VCC</t>
+  </si>
+  <si>
+    <t>power (3.3V)</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>i2c SDA OR SPI: MOSI</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>i2c &amp; SPI serial clock</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>DEN</t>
+  </si>
+  <si>
+    <t>gyroscope data enable</t>
+  </si>
+  <si>
+    <t>INT1</t>
+  </si>
+  <si>
+    <t>accel/gyro interrupt 1</t>
+  </si>
+  <si>
+    <t>INT2</t>
+  </si>
+  <si>
+    <t>accel/gyro interrupt 2</t>
+  </si>
+  <si>
+    <t>INTM</t>
+  </si>
+  <si>
+    <t>magnetometer interrupt</t>
+  </si>
+  <si>
+    <t>RDY</t>
+  </si>
+  <si>
+    <t>magnetometer data ready</t>
+  </si>
+  <si>
+    <t>CS M</t>
+  </si>
+  <si>
+    <t>magnetometer chip select</t>
+  </si>
+  <si>
+    <t>CS AG</t>
+  </si>
+  <si>
+    <t>Accel/Gyro chip select</t>
+  </si>
+  <si>
+    <t>SDO M</t>
+  </si>
+  <si>
+    <t>SPI: Magnetometer MISO,
+I2C: Magnetometer Address Select</t>
+  </si>
+  <si>
+    <t>SDO AG</t>
+  </si>
+  <si>
+    <t>SPI: Accel/Gyro MISO,
+I2C: Accel/Gryo Address Select</t>
+  </si>
+  <si>
+    <t>IMU</t>
+  </si>
+  <si>
+    <t>0.1" standard header pins</t>
+  </si>
+  <si>
+    <t>(only using this header)</t>
   </si>
 </sst>
 </file>
@@ -552,7 +642,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -656,18 +746,28 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -683,16 +783,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1008,13 +1101,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1069,7 +1162,7 @@
       <c r="C2" s="19">
         <v>1</v>
       </c>
-      <c r="D2" s="51"/>
+      <c r="D2" s="56"/>
       <c r="G2" s="37" t="s">
         <v>83</v>
       </c>
@@ -1086,7 +1179,7 @@
         <v>85</v>
       </c>
       <c r="C3" s="21"/>
-      <c r="D3" s="54"/>
+      <c r="D3" s="57"/>
       <c r="G3" s="38" t="s">
         <v>84</v>
       </c>
@@ -1101,7 +1194,7 @@
       <c r="A4" s="3"/>
       <c r="B4" s="9"/>
       <c r="C4" s="21"/>
-      <c r="D4" s="54"/>
+      <c r="D4" s="57"/>
       <c r="G4" s="3" t="s">
         <v>86</v>
       </c>
@@ -1115,7 +1208,7 @@
     <row r="5" spans="1:9" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
       <c r="C5" s="20"/>
-      <c r="D5" s="52"/>
+      <c r="D5" s="58"/>
       <c r="G5" s="5" t="s">
         <v>87</v>
       </c>
@@ -1133,7 +1226,7 @@
       <c r="C6" s="21">
         <v>1</v>
       </c>
-      <c r="D6" s="53"/>
+      <c r="D6" s="54"/>
       <c r="E6" s="4" t="s">
         <v>70</v>
       </c>
@@ -1151,7 +1244,7 @@
     <row r="7" spans="1:9" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="3"/>
       <c r="C7" s="21"/>
-      <c r="D7" s="60"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="4" t="s">
         <v>71</v>
       </c>
@@ -1171,7 +1264,7 @@
       <c r="C8" s="19">
         <v>1</v>
       </c>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="63" t="s">
         <v>80</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -1180,7 +1273,7 @@
       <c r="F8" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G8" s="63" t="s">
+      <c r="G8" s="51" t="s">
         <v>96</v>
       </c>
       <c r="H8" s="24" t="s">
@@ -1191,7 +1284,7 @@
     <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3"/>
       <c r="C9" s="21"/>
-      <c r="D9" s="56"/>
+      <c r="D9" s="60"/>
       <c r="E9" s="8" t="s">
         <v>3</v>
       </c>
@@ -1205,7 +1298,7 @@
     <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3"/>
       <c r="C10" s="21"/>
-      <c r="D10" s="61" t="s">
+      <c r="D10" s="52" t="s">
         <v>94</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -1221,7 +1314,7 @@
     <row r="11" spans="1:9" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="5"/>
       <c r="C11" s="20"/>
-      <c r="D11" s="62"/>
+      <c r="D11" s="53"/>
       <c r="E11" s="6" t="s">
         <v>1</v>
       </c>
@@ -1242,7 +1335,7 @@
       <c r="C12" s="19">
         <v>6</v>
       </c>
-      <c r="D12" s="51"/>
+      <c r="D12" s="56"/>
       <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1260,7 +1353,7 @@
     <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3"/>
       <c r="C13" s="21"/>
-      <c r="D13" s="54"/>
+      <c r="D13" s="57"/>
       <c r="E13" s="8" t="s">
         <v>10</v>
       </c>
@@ -1274,7 +1367,7 @@
     <row r="14" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3"/>
       <c r="C14" s="21"/>
-      <c r="D14" s="54"/>
+      <c r="D14" s="57"/>
       <c r="E14" s="8" t="s">
         <v>8</v>
       </c>
@@ -1288,7 +1381,7 @@
     <row r="15" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3"/>
       <c r="C15" s="21"/>
-      <c r="D15" s="54"/>
+      <c r="D15" s="57"/>
       <c r="E15" s="8" t="s">
         <v>11</v>
       </c>
@@ -1302,7 +1395,7 @@
     <row r="16" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3"/>
       <c r="C16" s="21"/>
-      <c r="D16" s="54"/>
+      <c r="D16" s="57"/>
       <c r="E16" s="8" t="s">
         <v>12</v>
       </c>
@@ -1316,7 +1409,7 @@
     <row r="17" spans="1:9" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="5"/>
       <c r="C17" s="20"/>
-      <c r="D17" s="52"/>
+      <c r="D17" s="58"/>
       <c r="E17" s="6" t="s">
         <v>13</v>
       </c>
@@ -1337,7 +1430,7 @@
       <c r="C18" s="32">
         <v>3</v>
       </c>
-      <c r="D18" s="59" t="s">
+      <c r="D18" s="63" t="s">
         <v>81</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -1357,7 +1450,7 @@
     <row r="19" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A19" s="3"/>
       <c r="C19" s="21"/>
-      <c r="D19" s="56"/>
+      <c r="D19" s="60"/>
       <c r="E19" s="4" t="s">
         <v>19</v>
       </c>
@@ -1371,7 +1464,7 @@
     <row r="20" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3"/>
       <c r="C20" s="21"/>
-      <c r="D20" s="56"/>
+      <c r="D20" s="60"/>
       <c r="E20" s="4" t="s">
         <v>20</v>
       </c>
@@ -1385,7 +1478,7 @@
     <row r="21" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3"/>
       <c r="C21" s="21"/>
-      <c r="D21" s="56"/>
+      <c r="D21" s="60"/>
       <c r="E21" s="4" t="s">
         <v>21</v>
       </c>
@@ -1400,7 +1493,7 @@
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
       <c r="C22" s="21"/>
-      <c r="D22" s="57"/>
+      <c r="D22" s="61"/>
       <c r="E22" s="15" t="s">
         <v>3</v>
       </c>
@@ -1415,7 +1508,7 @@
       <c r="A23" s="3"/>
       <c r="B23" s="25"/>
       <c r="C23" s="40"/>
-      <c r="D23" s="55" t="s">
+      <c r="D23" s="59" t="s">
         <v>80</v>
       </c>
       <c r="E23" s="12" t="s">
@@ -1435,7 +1528,7 @@
     <row r="24" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3"/>
       <c r="C24" s="21"/>
-      <c r="D24" s="56"/>
+      <c r="D24" s="60"/>
       <c r="E24" s="8" t="s">
         <v>33</v>
       </c>
@@ -1451,7 +1544,7 @@
     <row r="25" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3"/>
       <c r="C25" s="21"/>
-      <c r="D25" s="56"/>
+      <c r="D25" s="60"/>
       <c r="E25" s="8" t="s">
         <v>34</v>
       </c>
@@ -1469,7 +1562,7 @@
     <row r="26" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3"/>
       <c r="C26" s="21"/>
-      <c r="D26" s="56"/>
+      <c r="D26" s="60"/>
       <c r="E26" s="8" t="s">
         <v>35</v>
       </c>
@@ -1483,7 +1576,7 @@
     <row r="27" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3"/>
       <c r="C27" s="21"/>
-      <c r="D27" s="56"/>
+      <c r="D27" s="60"/>
       <c r="E27" s="8" t="s">
         <v>36</v>
       </c>
@@ -1501,7 +1594,7 @@
     <row r="28" spans="1:9" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A28" s="5"/>
       <c r="C28" s="20"/>
-      <c r="D28" s="58"/>
+      <c r="D28" s="62"/>
       <c r="E28" s="6" t="s">
         <v>37</v>
       </c>
@@ -1522,7 +1615,7 @@
       <c r="C29" s="32">
         <v>3</v>
       </c>
-      <c r="D29" s="55" t="s">
+      <c r="D29" s="59" t="s">
         <v>64</v>
       </c>
       <c r="E29" s="13" t="s">
@@ -1542,7 +1635,7 @@
     <row r="30" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="3"/>
       <c r="C30" s="33"/>
-      <c r="D30" s="56"/>
+      <c r="D30" s="60"/>
       <c r="E30" s="8" t="s">
         <v>45</v>
       </c>
@@ -1556,7 +1649,7 @@
     <row r="31" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="3"/>
       <c r="C31" s="21"/>
-      <c r="D31" s="56"/>
+      <c r="D31" s="60"/>
       <c r="E31" s="8" t="s">
         <v>46</v>
       </c>
@@ -1570,7 +1663,7 @@
     <row r="32" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A32" s="3"/>
       <c r="C32" s="21"/>
-      <c r="D32" s="56"/>
+      <c r="D32" s="60"/>
       <c r="E32" s="8" t="s">
         <v>3</v>
       </c>
@@ -1584,7 +1677,7 @@
     <row r="33" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A33" s="3"/>
       <c r="C33" s="21"/>
-      <c r="D33" s="56"/>
+      <c r="D33" s="60"/>
       <c r="E33" s="8" t="s">
         <v>47</v>
       </c>
@@ -1599,7 +1692,7 @@
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
       <c r="C34" s="21"/>
-      <c r="D34" s="57"/>
+      <c r="D34" s="61"/>
       <c r="E34" s="16" t="s">
         <v>48</v>
       </c>
@@ -1613,7 +1706,7 @@
     <row r="35" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A35" s="3"/>
       <c r="C35" s="21"/>
-      <c r="D35" s="55" t="s">
+      <c r="D35" s="59" t="s">
         <v>65</v>
       </c>
       <c r="E35" s="8" t="s">
@@ -1633,7 +1726,7 @@
     <row r="36" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="3"/>
       <c r="C36" s="21"/>
-      <c r="D36" s="56"/>
+      <c r="D36" s="60"/>
       <c r="E36" s="8" t="s">
         <v>53</v>
       </c>
@@ -1647,7 +1740,7 @@
     <row r="37" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A37" s="3"/>
       <c r="C37" s="21"/>
-      <c r="D37" s="56"/>
+      <c r="D37" s="60"/>
       <c r="E37" s="8" t="s">
         <v>54</v>
       </c>
@@ -1661,7 +1754,7 @@
     <row r="38" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="3"/>
       <c r="C38" s="21"/>
-      <c r="D38" s="56"/>
+      <c r="D38" s="60"/>
       <c r="E38" s="8" t="s">
         <v>3</v>
       </c>
@@ -1675,7 +1768,7 @@
     <row r="39" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A39" s="3"/>
       <c r="C39" s="21"/>
-      <c r="D39" s="56"/>
+      <c r="D39" s="60"/>
       <c r="E39" s="8" t="s">
         <v>55</v>
       </c>
@@ -1689,7 +1782,7 @@
     <row r="40" spans="1:9" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A40" s="5"/>
       <c r="C40" s="20"/>
-      <c r="D40" s="58"/>
+      <c r="D40" s="62"/>
       <c r="E40" s="6" t="s">
         <v>56</v>
       </c>
@@ -1700,8 +1793,214 @@
       <c r="H40" s="41"/>
       <c r="I40" s="30"/>
     </row>
+    <row r="41" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" s="19">
+        <v>1</v>
+      </c>
+      <c r="D41" s="63" t="s">
+        <v>101</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="I41" s="29"/>
+    </row>
+    <row r="42" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="47"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="H42" s="42"/>
+      <c r="I42" s="31"/>
+    </row>
+    <row r="43" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="3"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G43" s="3"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="31"/>
+    </row>
+    <row r="44" spans="1:9" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="3"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="61"/>
+      <c r="E44" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="G44" s="5"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="30"/>
+    </row>
+    <row r="45" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="3"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="59" t="s">
+        <v>108</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H45" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I45" s="31"/>
+    </row>
+    <row r="46" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="3"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G46" s="3"/>
+      <c r="H46" s="42"/>
+      <c r="I46" s="31"/>
+    </row>
+    <row r="47" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="3"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="60"/>
+      <c r="E47" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G47" s="3"/>
+      <c r="H47" s="42"/>
+      <c r="I47" s="31"/>
+    </row>
+    <row r="48" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="3"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="60"/>
+      <c r="E48" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G48" s="3"/>
+      <c r="H48" s="42"/>
+      <c r="I48" s="31"/>
+    </row>
+    <row r="49" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="3"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="60"/>
+      <c r="E49" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G49" s="3"/>
+      <c r="H49" s="42"/>
+      <c r="I49" s="31"/>
+    </row>
+    <row r="50" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="3"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="60"/>
+      <c r="E50" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G50" s="3"/>
+      <c r="H50" s="42"/>
+      <c r="I50" s="31"/>
+    </row>
+    <row r="51" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="3"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="60"/>
+      <c r="E51" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G51" s="3"/>
+      <c r="H51" s="42"/>
+      <c r="I51" s="31"/>
+    </row>
+    <row r="52" spans="1:9" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A52" s="3"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="60"/>
+      <c r="E52" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="G52" s="3"/>
+      <c r="H52" s="42"/>
+      <c r="I52" s="31"/>
+    </row>
+    <row r="53" spans="1:9" s="6" customFormat="1" ht="29.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="5"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="62"/>
+      <c r="E53" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F53" s="64" t="s">
+        <v>126</v>
+      </c>
+      <c r="G53" s="5"/>
+      <c r="H53" s="41"/>
+      <c r="I53" s="30"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
+    <mergeCell ref="D41:D44"/>
+    <mergeCell ref="D45:D53"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D2:D5"/>
@@ -1727,8 +2026,11 @@
     <hyperlink ref="H23" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="H6" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="H8" r:id="rId14" xr:uid="{0E01A5F4-00F9-40BD-990F-C3B6F2273C64}"/>
+    <hyperlink ref="B41" r:id="rId15" xr:uid="{6FF516DD-2C53-4A64-B15A-40ECC7D4697C}"/>
+    <hyperlink ref="H41" r:id="rId16" xr:uid="{0F6BD004-63B1-4DF0-B6C7-19C11115895E}"/>
+    <hyperlink ref="H45" r:id="rId17" xr:uid="{0246C317-3E62-4679-8325-285F66C2CD4F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
not sure if i updated arduino connections recently but it said it changed
</commit_message>
<xml_diff>
--- a/Electrical/Arduino_ExternalConnections.xlsx
+++ b/Electrical/Arduino_ExternalConnections.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub_Local\2018\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC542083-4E6B-4F13-8530-56EB9B000040}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06830240-1ACD-431F-8461-0CB078213A3B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18574" yWindow="0" windowWidth="18523" windowHeight="10423" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19671" yWindow="0" windowWidth="18523" windowHeight="10423" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -747,6 +747,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -767,24 +785,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1104,10 +1104,10 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G43" sqref="G43"/>
+      <selection pane="bottomRight" activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1162,7 +1162,7 @@
       <c r="C2" s="19">
         <v>1</v>
       </c>
-      <c r="D2" s="56"/>
+      <c r="D2" s="62"/>
       <c r="G2" s="37" t="s">
         <v>83</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>85</v>
       </c>
       <c r="C3" s="21"/>
-      <c r="D3" s="57"/>
+      <c r="D3" s="63"/>
       <c r="G3" s="38" t="s">
         <v>84</v>
       </c>
@@ -1194,7 +1194,7 @@
       <c r="A4" s="3"/>
       <c r="B4" s="9"/>
       <c r="C4" s="21"/>
-      <c r="D4" s="57"/>
+      <c r="D4" s="63"/>
       <c r="G4" s="3" t="s">
         <v>86</v>
       </c>
@@ -1208,7 +1208,7 @@
     <row r="5" spans="1:9" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
       <c r="C5" s="20"/>
-      <c r="D5" s="58"/>
+      <c r="D5" s="64"/>
       <c r="G5" s="5" t="s">
         <v>87</v>
       </c>
@@ -1226,7 +1226,7 @@
       <c r="C6" s="21">
         <v>1</v>
       </c>
-      <c r="D6" s="54"/>
+      <c r="D6" s="60"/>
       <c r="E6" s="4" t="s">
         <v>70</v>
       </c>
@@ -1244,7 +1244,7 @@
     <row r="7" spans="1:9" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="3"/>
       <c r="C7" s="21"/>
-      <c r="D7" s="55"/>
+      <c r="D7" s="61"/>
       <c r="E7" s="4" t="s">
         <v>71</v>
       </c>
@@ -1264,7 +1264,7 @@
       <c r="C8" s="19">
         <v>1</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="53" t="s">
         <v>80</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -1284,7 +1284,7 @@
     <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3"/>
       <c r="C9" s="21"/>
-      <c r="D9" s="60"/>
+      <c r="D9" s="54"/>
       <c r="E9" s="8" t="s">
         <v>3</v>
       </c>
@@ -1298,7 +1298,7 @@
     <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3"/>
       <c r="C10" s="21"/>
-      <c r="D10" s="52" t="s">
+      <c r="D10" s="58" t="s">
         <v>94</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -1314,7 +1314,7 @@
     <row r="11" spans="1:9" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="5"/>
       <c r="C11" s="20"/>
-      <c r="D11" s="53"/>
+      <c r="D11" s="59"/>
       <c r="E11" s="6" t="s">
         <v>1</v>
       </c>
@@ -1335,7 +1335,7 @@
       <c r="C12" s="19">
         <v>6</v>
       </c>
-      <c r="D12" s="56"/>
+      <c r="D12" s="62"/>
       <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1353,7 +1353,7 @@
     <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3"/>
       <c r="C13" s="21"/>
-      <c r="D13" s="57"/>
+      <c r="D13" s="63"/>
       <c r="E13" s="8" t="s">
         <v>10</v>
       </c>
@@ -1367,7 +1367,7 @@
     <row r="14" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3"/>
       <c r="C14" s="21"/>
-      <c r="D14" s="57"/>
+      <c r="D14" s="63"/>
       <c r="E14" s="8" t="s">
         <v>8</v>
       </c>
@@ -1381,7 +1381,7 @@
     <row r="15" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3"/>
       <c r="C15" s="21"/>
-      <c r="D15" s="57"/>
+      <c r="D15" s="63"/>
       <c r="E15" s="8" t="s">
         <v>11</v>
       </c>
@@ -1395,7 +1395,7 @@
     <row r="16" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3"/>
       <c r="C16" s="21"/>
-      <c r="D16" s="57"/>
+      <c r="D16" s="63"/>
       <c r="E16" s="8" t="s">
         <v>12</v>
       </c>
@@ -1409,7 +1409,7 @@
     <row r="17" spans="1:9" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="5"/>
       <c r="C17" s="20"/>
-      <c r="D17" s="58"/>
+      <c r="D17" s="64"/>
       <c r="E17" s="6" t="s">
         <v>13</v>
       </c>
@@ -1430,7 +1430,7 @@
       <c r="C18" s="32">
         <v>3</v>
       </c>
-      <c r="D18" s="63" t="s">
+      <c r="D18" s="53" t="s">
         <v>81</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -1450,7 +1450,7 @@
     <row r="19" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A19" s="3"/>
       <c r="C19" s="21"/>
-      <c r="D19" s="60"/>
+      <c r="D19" s="54"/>
       <c r="E19" s="4" t="s">
         <v>19</v>
       </c>
@@ -1464,7 +1464,7 @@
     <row r="20" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3"/>
       <c r="C20" s="21"/>
-      <c r="D20" s="60"/>
+      <c r="D20" s="54"/>
       <c r="E20" s="4" t="s">
         <v>20</v>
       </c>
@@ -1478,7 +1478,7 @@
     <row r="21" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3"/>
       <c r="C21" s="21"/>
-      <c r="D21" s="60"/>
+      <c r="D21" s="54"/>
       <c r="E21" s="4" t="s">
         <v>21</v>
       </c>
@@ -1493,7 +1493,7 @@
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
       <c r="C22" s="21"/>
-      <c r="D22" s="61"/>
+      <c r="D22" s="55"/>
       <c r="E22" s="15" t="s">
         <v>3</v>
       </c>
@@ -1508,7 +1508,7 @@
       <c r="A23" s="3"/>
       <c r="B23" s="25"/>
       <c r="C23" s="40"/>
-      <c r="D23" s="59" t="s">
+      <c r="D23" s="56" t="s">
         <v>80</v>
       </c>
       <c r="E23" s="12" t="s">
@@ -1528,7 +1528,7 @@
     <row r="24" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3"/>
       <c r="C24" s="21"/>
-      <c r="D24" s="60"/>
+      <c r="D24" s="54"/>
       <c r="E24" s="8" t="s">
         <v>33</v>
       </c>
@@ -1544,7 +1544,7 @@
     <row r="25" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3"/>
       <c r="C25" s="21"/>
-      <c r="D25" s="60"/>
+      <c r="D25" s="54"/>
       <c r="E25" s="8" t="s">
         <v>34</v>
       </c>
@@ -1562,7 +1562,7 @@
     <row r="26" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3"/>
       <c r="C26" s="21"/>
-      <c r="D26" s="60"/>
+      <c r="D26" s="54"/>
       <c r="E26" s="8" t="s">
         <v>35</v>
       </c>
@@ -1576,7 +1576,7 @@
     <row r="27" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3"/>
       <c r="C27" s="21"/>
-      <c r="D27" s="60"/>
+      <c r="D27" s="54"/>
       <c r="E27" s="8" t="s">
         <v>36</v>
       </c>
@@ -1594,7 +1594,7 @@
     <row r="28" spans="1:9" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A28" s="5"/>
       <c r="C28" s="20"/>
-      <c r="D28" s="62"/>
+      <c r="D28" s="57"/>
       <c r="E28" s="6" t="s">
         <v>37</v>
       </c>
@@ -1615,7 +1615,7 @@
       <c r="C29" s="32">
         <v>3</v>
       </c>
-      <c r="D29" s="59" t="s">
+      <c r="D29" s="56" t="s">
         <v>64</v>
       </c>
       <c r="E29" s="13" t="s">
@@ -1635,7 +1635,7 @@
     <row r="30" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="3"/>
       <c r="C30" s="33"/>
-      <c r="D30" s="60"/>
+      <c r="D30" s="54"/>
       <c r="E30" s="8" t="s">
         <v>45</v>
       </c>
@@ -1649,7 +1649,7 @@
     <row r="31" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="3"/>
       <c r="C31" s="21"/>
-      <c r="D31" s="60"/>
+      <c r="D31" s="54"/>
       <c r="E31" s="8" t="s">
         <v>46</v>
       </c>
@@ -1663,7 +1663,7 @@
     <row r="32" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A32" s="3"/>
       <c r="C32" s="21"/>
-      <c r="D32" s="60"/>
+      <c r="D32" s="54"/>
       <c r="E32" s="8" t="s">
         <v>3</v>
       </c>
@@ -1677,7 +1677,7 @@
     <row r="33" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A33" s="3"/>
       <c r="C33" s="21"/>
-      <c r="D33" s="60"/>
+      <c r="D33" s="54"/>
       <c r="E33" s="8" t="s">
         <v>47</v>
       </c>
@@ -1692,7 +1692,7 @@
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
       <c r="C34" s="21"/>
-      <c r="D34" s="61"/>
+      <c r="D34" s="55"/>
       <c r="E34" s="16" t="s">
         <v>48</v>
       </c>
@@ -1706,7 +1706,7 @@
     <row r="35" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A35" s="3"/>
       <c r="C35" s="21"/>
-      <c r="D35" s="59" t="s">
+      <c r="D35" s="56" t="s">
         <v>65</v>
       </c>
       <c r="E35" s="8" t="s">
@@ -1726,7 +1726,7 @@
     <row r="36" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="3"/>
       <c r="C36" s="21"/>
-      <c r="D36" s="60"/>
+      <c r="D36" s="54"/>
       <c r="E36" s="8" t="s">
         <v>53</v>
       </c>
@@ -1740,7 +1740,7 @@
     <row r="37" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A37" s="3"/>
       <c r="C37" s="21"/>
-      <c r="D37" s="60"/>
+      <c r="D37" s="54"/>
       <c r="E37" s="8" t="s">
         <v>54</v>
       </c>
@@ -1754,7 +1754,7 @@
     <row r="38" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="3"/>
       <c r="C38" s="21"/>
-      <c r="D38" s="60"/>
+      <c r="D38" s="54"/>
       <c r="E38" s="8" t="s">
         <v>3</v>
       </c>
@@ -1768,7 +1768,7 @@
     <row r="39" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A39" s="3"/>
       <c r="C39" s="21"/>
-      <c r="D39" s="60"/>
+      <c r="D39" s="54"/>
       <c r="E39" s="8" t="s">
         <v>55</v>
       </c>
@@ -1782,7 +1782,7 @@
     <row r="40" spans="1:9" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A40" s="5"/>
       <c r="C40" s="20"/>
-      <c r="D40" s="62"/>
+      <c r="D40" s="57"/>
       <c r="E40" s="6" t="s">
         <v>56</v>
       </c>
@@ -1803,7 +1803,7 @@
       <c r="C41" s="19">
         <v>1</v>
       </c>
-      <c r="D41" s="63" t="s">
+      <c r="D41" s="53" t="s">
         <v>101</v>
       </c>
       <c r="E41" s="2" t="s">
@@ -1824,7 +1824,7 @@
       <c r="A42" s="47"/>
       <c r="B42" s="9"/>
       <c r="C42" s="21"/>
-      <c r="D42" s="60"/>
+      <c r="D42" s="54"/>
       <c r="E42" s="4" t="s">
         <v>102</v>
       </c>
@@ -1840,7 +1840,7 @@
     <row r="43" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A43" s="3"/>
       <c r="C43" s="21"/>
-      <c r="D43" s="60"/>
+      <c r="D43" s="54"/>
       <c r="E43" s="4" t="s">
         <v>104</v>
       </c>
@@ -1854,7 +1854,7 @@
     <row r="44" spans="1:9" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A44" s="3"/>
       <c r="C44" s="21"/>
-      <c r="D44" s="61"/>
+      <c r="D44" s="55"/>
       <c r="E44" s="15" t="s">
         <v>106</v>
       </c>
@@ -1868,7 +1868,7 @@
     <row r="45" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A45" s="3"/>
       <c r="C45" s="21"/>
-      <c r="D45" s="59" t="s">
+      <c r="D45" s="56" t="s">
         <v>108</v>
       </c>
       <c r="E45" s="12" t="s">
@@ -1888,7 +1888,7 @@
     <row r="46" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A46" s="3"/>
       <c r="C46" s="21"/>
-      <c r="D46" s="60"/>
+      <c r="D46" s="54"/>
       <c r="E46" s="4" t="s">
         <v>111</v>
       </c>
@@ -1902,7 +1902,7 @@
     <row r="47" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A47" s="3"/>
       <c r="C47" s="21"/>
-      <c r="D47" s="60"/>
+      <c r="D47" s="54"/>
       <c r="E47" s="4" t="s">
         <v>113</v>
       </c>
@@ -1916,7 +1916,7 @@
     <row r="48" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A48" s="3"/>
       <c r="C48" s="21"/>
-      <c r="D48" s="60"/>
+      <c r="D48" s="54"/>
       <c r="E48" s="4" t="s">
         <v>115</v>
       </c>
@@ -1930,7 +1930,7 @@
     <row r="49" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A49" s="3"/>
       <c r="C49" s="21"/>
-      <c r="D49" s="60"/>
+      <c r="D49" s="54"/>
       <c r="E49" s="4" t="s">
         <v>117</v>
       </c>
@@ -1944,7 +1944,7 @@
     <row r="50" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A50" s="3"/>
       <c r="C50" s="21"/>
-      <c r="D50" s="60"/>
+      <c r="D50" s="54"/>
       <c r="E50" s="4" t="s">
         <v>119</v>
       </c>
@@ -1958,7 +1958,7 @@
     <row r="51" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A51" s="3"/>
       <c r="C51" s="21"/>
-      <c r="D51" s="60"/>
+      <c r="D51" s="54"/>
       <c r="E51" s="4" t="s">
         <v>121</v>
       </c>
@@ -1972,7 +1972,7 @@
     <row r="52" spans="1:9" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A52" s="3"/>
       <c r="C52" s="21"/>
-      <c r="D52" s="60"/>
+      <c r="D52" s="54"/>
       <c r="E52" s="4" t="s">
         <v>123</v>
       </c>
@@ -1986,11 +1986,11 @@
     <row r="53" spans="1:9" s="6" customFormat="1" ht="29.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A53" s="5"/>
       <c r="C53" s="20"/>
-      <c r="D53" s="62"/>
+      <c r="D53" s="57"/>
       <c r="E53" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="F53" s="64" t="s">
+      <c r="F53" s="52" t="s">
         <v>126</v>
       </c>
       <c r="G53" s="5"/>

</xml_diff>